<commit_message>
📊 Update NAIC content history - 2026-01-06
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4235514-040E-40F0-9AB6-6BAC02F98698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9573ED03-C958-41BB-8AED-27FFBCCFC786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2078,51 +2078,51 @@
           <cell r="H7">
             <v>46025</v>
           </cell>
-          <cell r="I7" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J7" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K7" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L7" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I7">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J7">
+            <v>4.3200000000000002E-2</v>
+          </cell>
+          <cell r="K7">
+            <v>4.5900000000000003E-2</v>
+          </cell>
+          <cell r="L7">
+            <v>4.8800000000000003E-2</v>
           </cell>
         </row>
         <row r="8">
           <cell r="H8">
             <v>46026</v>
           </cell>
-          <cell r="I8" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J8" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K8" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L8" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I8">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J8">
+            <v>4.3200000000000002E-2</v>
+          </cell>
+          <cell r="K8">
+            <v>4.5900000000000003E-2</v>
+          </cell>
+          <cell r="L8">
+            <v>4.8800000000000003E-2</v>
           </cell>
         </row>
         <row r="9">
           <cell r="H9">
             <v>46027</v>
           </cell>
-          <cell r="I9" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J9" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K9" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L9" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I9">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J9">
+            <v>4.3200000000000002E-2</v>
+          </cell>
+          <cell r="K9">
+            <v>4.5900000000000003E-2</v>
+          </cell>
+          <cell r="L9">
+            <v>4.8800000000000003E-2</v>
           </cell>
         </row>
         <row r="10">
@@ -8563,16 +8563,16 @@
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,73 +8651,73 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
       </c>
-      <c r="B6" s="17" t="str">
+      <c r="B6" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C6" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C6" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D6" s="47" t="str">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="D6" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E6" s="5" t="str">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="E6" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L7</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
       </c>
-      <c r="B7" s="17" t="str">
+      <c r="B7" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C7" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D7" s="47" t="str">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="D7" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E7" s="5" t="str">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="E7" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L8</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
       </c>
-      <c r="B8" s="17" t="str">
+      <c r="B8" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C8" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C8" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D8" s="47" t="str">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="D8" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E8" s="5" t="str">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="E8" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L9</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-07
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9573ED03-C958-41BB-8AED-27FFBCCFC786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA868E-E437-44A6-B25F-BF5ED3368094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2129,17 +2129,17 @@
           <cell r="H10">
             <v>46028</v>
           </cell>
-          <cell r="I10" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J10" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K10" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L10" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I10">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J10">
+            <v>4.2900000000000001E-2</v>
+          </cell>
+          <cell r="K10">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L10">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="11">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,29 +8717,29 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
       </c>
-      <c r="B9" s="17" t="str">
+      <c r="B9" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C9" s="47" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C9" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D9" s="47" t="str">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D9" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E9" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E9" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L10</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16707,16 +16707,16 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16874,16 +16874,16 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17515,196 +17515,196 @@
   <dimension ref="A1:AU36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-08
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA868E-E437-44A6-B25F-BF5ED3368094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6130AE1-4FB0-4772-9C4F-38067169125F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34425" yWindow="2535" windowWidth="20370" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2146,17 +2146,17 @@
           <cell r="H11">
             <v>46029</v>
           </cell>
-          <cell r="I11" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J11" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K11" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L11" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I11">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J11">
+            <v>4.2900000000000001E-2</v>
+          </cell>
+          <cell r="K11">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L11">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="12">
@@ -8744,21 +8744,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
       </c>
-      <c r="B10" s="17" t="str">
+      <c r="B10" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I11</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C10" s="47" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C10" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J11</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D10" s="47" t="str">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D10" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K11</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E10" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E10" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L11</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8500000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17527,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="str" cm="1">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-09
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6130AE1-4FB0-4772-9C4F-38067169125F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC23C80-7290-42F7-B4EE-95AAC03BA60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34425" yWindow="2535" windowWidth="20370" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2163,17 +2163,17 @@
           <cell r="H12">
             <v>46030</v>
           </cell>
-          <cell r="I12" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J12" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K12" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L12" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I12">
+            <v>3.9199999999999999E-2</v>
+          </cell>
+          <cell r="J12">
+            <v>4.2700000000000002E-2</v>
+          </cell>
+          <cell r="K12">
+            <v>4.5400000000000003E-2</v>
+          </cell>
+          <cell r="L12">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="13">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,29 +8761,29 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
       </c>
-      <c r="B11" s="17" t="str">
+      <c r="B11" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I12</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="47" t="str">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="C11" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J12</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D11" s="47" t="str">
+        <v>4.2700000000000002E-2</v>
+      </c>
+      <c r="D11" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K12</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E11" s="5" t="str">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E11" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L12</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-10
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC23C80-7290-42F7-B4EE-95AAC03BA60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFC368-6B22-488C-83C5-289F3CC09512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="555" windowWidth="26625" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2180,17 +2180,17 @@
           <cell r="H13">
             <v>46031</v>
           </cell>
-          <cell r="I13" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J13" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K13" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L13" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I13">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J13">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K13">
+            <v>4.58E-2</v>
+          </cell>
+          <cell r="L13">
+            <v>4.8599999999999997E-2</v>
           </cell>
         </row>
         <row r="14">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,29 +8783,29 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
       </c>
-      <c r="B12" s="17" t="str">
+      <c r="B12" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I13</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C12" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J13</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D12" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D12" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K13</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E12" s="5" t="str">
+        <v>4.58E-2</v>
+      </c>
+      <c r="E12" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L13</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.8599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-13
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFC368-6B22-488C-83C5-289F3CC09512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D6E2B-919D-4C8D-9882-EF35B7ADFA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="555" windowWidth="26625" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2197,51 +2197,51 @@
           <cell r="H14">
             <v>46032</v>
           </cell>
-          <cell r="I14" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J14" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K14" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L14" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I14">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J14">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K14">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L14">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="15">
           <cell r="H15">
             <v>46033</v>
           </cell>
-          <cell r="I15" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J15" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K15" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L15" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I15">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J15">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K15">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L15">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="16">
           <cell r="H16">
             <v>46034</v>
           </cell>
-          <cell r="I16" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J16" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K16" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L16" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I16">
+            <v>3.9600000000000003E-2</v>
+          </cell>
+          <cell r="J16">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K16">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L16">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="17">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,73 +8805,73 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
       </c>
-      <c r="B13" s="49" t="str">
+      <c r="B13" s="49">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I14</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C13" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J14</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D13" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D13" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K14</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E13" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E13" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L14</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
       </c>
-      <c r="B14" s="17" t="str">
+      <c r="B14" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I15</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C14" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J15</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D14" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D14" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K15</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E14" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E14" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L15</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
       </c>
-      <c r="B15" s="17" t="str">
+      <c r="B15" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="47" t="str">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C15" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D15" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D15" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E15" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E15" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L16</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-14
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D6E2B-919D-4C8D-9882-EF35B7ADFA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F51DA7-D64A-4A76-93A8-E66D8A70522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2248,17 +2248,17 @@
           <cell r="H17">
             <v>46035</v>
           </cell>
-          <cell r="I17" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J17" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K17" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L17" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I17">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J17">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K17">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L17">
+            <v>4.8399999999999999E-2</v>
           </cell>
         </row>
         <row r="18">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,29 +8871,29 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
       </c>
-      <c r="B16" s="17" t="str">
+      <c r="B16" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I17</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C16" s="47" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C16" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J17</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D16" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D16" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K17</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E16" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E16" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L17</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.8399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-16
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F51DA7-D64A-4A76-93A8-E66D8A70522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2104BF-2803-4138-9763-9F55FBBD744A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2265,34 +2265,34 @@
           <cell r="H18">
             <v>46036</v>
           </cell>
-          <cell r="I18" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J18" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K18" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L18" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I18">
+            <v>3.9399999999999998E-2</v>
+          </cell>
+          <cell r="J18">
+            <v>4.2900000000000001E-2</v>
+          </cell>
+          <cell r="K18">
+            <v>4.5499999999999999E-2</v>
+          </cell>
+          <cell r="L18">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="19">
           <cell r="H19">
             <v>46037</v>
           </cell>
-          <cell r="I19" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J19" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K19" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L19" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I19">
+            <v>3.9199999999999999E-2</v>
+          </cell>
+          <cell r="J19">
+            <v>4.2500000000000003E-2</v>
+          </cell>
+          <cell r="K19">
+            <v>4.5199999999999997E-2</v>
+          </cell>
+          <cell r="L19">
+            <v>4.7899999999999998E-2</v>
           </cell>
         </row>
         <row r="20">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,51 +8893,51 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
       </c>
-      <c r="B17" s="17" t="str">
+      <c r="B17" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C17" s="47" t="str">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="C17" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D17" s="47" t="str">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D17" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E17" s="5" t="str">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E17" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L18</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
       </c>
-      <c r="B18" s="17" t="str">
+      <c r="B18" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I19</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C18" s="47" t="str">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="C18" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J19</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D18" s="47" t="str">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="D18" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K19</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E18" s="5" t="str">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E18" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L19</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.7899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-17
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2104BF-2803-4138-9763-9F55FBBD744A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF873D65-87ED-4521-8810-E95B318856F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2299,17 +2299,17 @@
           <cell r="H20">
             <v>46038</v>
           </cell>
-          <cell r="I20" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J20" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K20" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L20" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I20">
+            <v>3.95E-2</v>
+          </cell>
+          <cell r="J20">
+            <v>4.2700000000000002E-2</v>
+          </cell>
+          <cell r="K20">
+            <v>4.53E-2</v>
+          </cell>
+          <cell r="L20">
+            <v>4.7899999999999998E-2</v>
           </cell>
         </row>
         <row r="21">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,29 +8937,29 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
       </c>
-      <c r="B19" s="17" t="str">
+      <c r="B19" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I20</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C19" s="47" t="str">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C19" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J20</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D19" s="47" t="str">
+        <v>4.2700000000000002E-2</v>
+      </c>
+      <c r="D19" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K20</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E19" s="5" t="str">
+        <v>4.53E-2</v>
+      </c>
+      <c r="E19" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L20</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.7899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-21
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF873D65-87ED-4521-8810-E95B318856F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA17B590-DC20-4EAA-BAFC-4A8719A81533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2316,68 +2316,68 @@
           <cell r="H21">
             <v>46039</v>
           </cell>
-          <cell r="I21" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J21" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K21" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L21" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I21">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J21">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K21">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L21">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="22">
           <cell r="H22">
             <v>46040</v>
           </cell>
-          <cell r="I22" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J22" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K22" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L22" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I22">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J22">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K22">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L22">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="23">
           <cell r="H23">
             <v>46041</v>
           </cell>
-          <cell r="I23" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J23" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K23" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L23" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I23">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J23">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K23">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L23">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="24">
           <cell r="H24">
             <v>46042</v>
           </cell>
-          <cell r="I24" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J24" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K24" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L24" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I24">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J24">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K24">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L24">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="25">
@@ -8560,7 +8560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8964,21 +8964,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
       </c>
-      <c r="B20" s="17" t="str">
+      <c r="B20" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I21</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C20" s="47" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C20" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J21</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D20" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D20" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K21</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E20" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E20" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L21</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -8986,21 +8986,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
       </c>
-      <c r="B21" s="17" t="str">
+      <c r="B21" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I22</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C21" s="47" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C21" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J22</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D21" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D21" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K22</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E21" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E21" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L22</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -9008,21 +9008,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
       </c>
-      <c r="B22" s="17" t="str">
+      <c r="B22" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I23</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C22" s="47" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C22" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J23</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D22" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D22" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K23</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E22" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E22" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L23</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -9030,21 +9030,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
       </c>
-      <c r="B23" s="17" t="str">
+      <c r="B23" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I24</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C23" s="47" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C23" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J24</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D23" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D23" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K24</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E23" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E23" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L24</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17527,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-22
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA17B590-DC20-4EAA-BAFC-4A8719A81533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D5ADA0-4306-40F5-9111-321646B52BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33585" yWindow="1680" windowWidth="20655" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2384,17 +2384,17 @@
           <cell r="H25">
             <v>46043</v>
           </cell>
-          <cell r="I25" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J25" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K25" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L25" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I25">
+            <v>4.0099999999999997E-2</v>
+          </cell>
+          <cell r="J25">
+            <v>4.36E-2</v>
+          </cell>
+          <cell r="K25">
+            <v>4.6300000000000001E-2</v>
+          </cell>
+          <cell r="L25">
+            <v>4.9000000000000002E-2</v>
           </cell>
         </row>
         <row r="26">
@@ -9052,21 +9052,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
       </c>
-      <c r="B24" s="17" t="str">
+      <c r="B24" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I25</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C24" s="47" t="str">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="C24" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J25</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D24" s="47" t="str">
+        <v>4.36E-2</v>
+      </c>
+      <c r="D24" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K25</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E24" s="5" t="str">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="E24" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L25</f>
-        <v xml:space="preserve"> </v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17527,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="str" cm="1">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-23
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D5ADA0-4306-40F5-9111-321646B52BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE233F7C-64E9-4F94-9095-8B16EA2C1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33585" yWindow="1680" windowWidth="20655" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2401,17 +2401,17 @@
           <cell r="H26">
             <v>46044</v>
           </cell>
-          <cell r="I26" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J26" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K26" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L26" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I26">
+            <v>3.9800000000000002E-2</v>
+          </cell>
+          <cell r="J26">
+            <v>4.3200000000000002E-2</v>
+          </cell>
+          <cell r="K26">
+            <v>4.58E-2</v>
+          </cell>
+          <cell r="L26">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="27">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,29 +9069,29 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
       </c>
-      <c r="B25" s="17" t="str">
+      <c r="B25" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I26</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C25" s="47" t="str">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="C25" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J26</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D25" s="47" t="str">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="D25" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K26</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E25" s="5" t="str">
+        <v>4.58E-2</v>
+      </c>
+      <c r="E25" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L26</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-24
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE233F7C-64E9-4F94-9095-8B16EA2C1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4398EA-C60E-42B4-BEF9-E5B0F0761103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2535" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31785" yWindow="1185" windowWidth="23715" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2418,17 +2418,17 @@
           <cell r="H27">
             <v>46045</v>
           </cell>
-          <cell r="I27" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J27" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K27" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L27" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I27">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J27">
+            <v>4.3099999999999999E-2</v>
+          </cell>
+          <cell r="K27">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L27">
+            <v>4.82E-2</v>
           </cell>
         </row>
         <row r="28">
@@ -8563,16 +8563,16 @@
       <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,29 +9091,29 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
       </c>
-      <c r="B26" s="17" t="str">
+      <c r="B26" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I27</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C26" s="47" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C26" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J27</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D26" s="47" t="str">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="D26" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K27</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E26" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E26" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L27</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.82E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,7 +9179,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-27
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4398EA-C60E-42B4-BEF9-E5B0F0761103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D3F5A-1833-4B42-986E-289EC4F6D0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31785" yWindow="1185" windowWidth="23715" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2435,51 +2435,51 @@
           <cell r="H28">
             <v>46046</v>
           </cell>
-          <cell r="I28" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J28" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K28" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L28" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I28">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J28">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K28">
+            <v>4.5499999999999999E-2</v>
+          </cell>
+          <cell r="L28">
+            <v>4.82E-2</v>
           </cell>
         </row>
         <row r="29">
           <cell r="H29">
             <v>46047</v>
           </cell>
-          <cell r="I29" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J29" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K29" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L29" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I29">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J29">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K29">
+            <v>4.5499999999999999E-2</v>
+          </cell>
+          <cell r="L29">
+            <v>4.82E-2</v>
           </cell>
         </row>
         <row r="30">
           <cell r="H30">
             <v>46048</v>
           </cell>
-          <cell r="I30" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J30" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K30" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L30" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I30">
+            <v>3.9699999999999999E-2</v>
+          </cell>
+          <cell r="J30">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K30">
+            <v>4.5499999999999999E-2</v>
+          </cell>
+          <cell r="L30">
+            <v>4.82E-2</v>
           </cell>
         </row>
         <row r="31">
@@ -8560,19 +8560,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,73 +9113,73 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
       </c>
-      <c r="B27" s="17" t="str">
+      <c r="B27" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I28</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C27" s="47" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C27" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J28</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D27" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D27" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K28</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E27" s="5" t="str">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E27" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L28</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.82E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
       </c>
-      <c r="B28" s="17" t="str">
+      <c r="B28" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I29</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C28" s="47" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C28" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J29</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D28" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D28" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K29</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E28" s="5" t="str">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E28" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L29</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.82E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
       </c>
-      <c r="B29" s="17" t="str">
+      <c r="B29" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I30</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C29" s="47" t="str">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C29" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J30</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D29" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D29" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K30</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E29" s="5" t="str">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E29" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L30</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.82E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9201,7 +9201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
+                <xdr:colOff>336550</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-28
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D3F5A-1833-4B42-986E-289EC4F6D0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D89A1B-3A78-412F-9B6B-3982D22484D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>336550</xdr:colOff>
+          <xdr:colOff>333375</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2486,17 +2486,17 @@
           <cell r="H31">
             <v>46049</v>
           </cell>
-          <cell r="I31" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J31" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K31" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L31" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I31">
+            <v>3.95E-2</v>
+          </cell>
+          <cell r="J31">
+            <v>4.2900000000000001E-2</v>
+          </cell>
+          <cell r="K31">
+            <v>4.5400000000000003E-2</v>
+          </cell>
+          <cell r="L31">
+            <v>4.8000000000000001E-2</v>
           </cell>
         </row>
         <row r="32">
@@ -8559,20 +8559,20 @@
   <dimension ref="A1:E380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8581,7 +8581,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8629,7 +8629,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8651,7 +8651,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8673,7 +8673,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8695,7 +8695,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8717,7 +8717,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8739,7 +8739,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8761,7 +8761,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8783,7 +8783,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8805,7 +8805,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8827,7 +8827,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8849,7 +8849,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8871,7 +8871,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8893,7 +8893,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8915,7 +8915,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8937,7 +8937,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8959,7 +8959,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8981,7 +8981,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9003,7 +9003,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9025,7 +9025,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9047,7 +9047,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9069,7 +9069,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9091,7 +9091,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9113,7 +9113,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9135,7 +9135,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9157,7 +9157,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9179,29 +9179,29 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
       </c>
-      <c r="B30" s="17" t="str">
+      <c r="B30" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I31</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C30" s="47" t="str">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C30" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J31</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D30" s="47" t="str">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D30" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K31</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E30" s="5" t="str">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E30" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L31</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9223,7 +9223,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9245,7 +9245,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9267,7 +9267,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
@@ -9289,7 +9289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
@@ -9311,7 +9311,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
@@ -9333,7 +9333,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9355,7 +9355,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9377,7 +9377,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9399,7 +9399,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9421,7 +9421,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9443,7 +9443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9465,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9487,7 +9487,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9509,7 +9509,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9531,7 +9531,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9553,7 +9553,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9575,7 +9575,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9597,7 +9597,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9619,7 +9619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9641,7 +9641,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9663,7 +9663,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9685,7 +9685,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9729,7 +9729,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9751,7 +9751,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9773,7 +9773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9795,7 +9795,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9817,7 +9817,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9839,7 +9839,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9861,7 +9861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9883,7 +9883,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9905,7 +9905,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9927,7 +9927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9949,7 +9949,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9971,7 +9971,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9993,7 +9993,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10015,7 +10015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10037,7 +10037,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10059,7 +10059,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10081,7 +10081,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10103,7 +10103,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10125,7 +10125,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10147,7 +10147,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10169,7 +10169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10191,7 +10191,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10213,7 +10213,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10235,7 +10235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10257,7 +10257,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10279,7 +10279,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10301,7 +10301,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10323,7 +10323,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10345,7 +10345,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10367,7 +10367,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10389,7 +10389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10411,7 +10411,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10433,7 +10433,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10455,7 +10455,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10477,7 +10477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10499,7 +10499,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10521,7 +10521,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10543,7 +10543,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10565,7 +10565,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10587,7 +10587,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10609,7 +10609,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10631,7 +10631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10653,7 +10653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10675,7 +10675,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10697,7 +10697,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10719,7 +10719,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10741,7 +10741,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10763,7 +10763,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10785,7 +10785,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10807,7 +10807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10829,7 +10829,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10851,7 +10851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10873,7 +10873,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10895,7 +10895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10917,7 +10917,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10939,7 +10939,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10983,7 +10983,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11005,7 +11005,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11027,7 +11027,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11049,7 +11049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11071,7 +11071,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11093,7 +11093,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11115,7 +11115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11137,7 +11137,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11159,7 +11159,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11181,7 +11181,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11225,7 +11225,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11247,7 +11247,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11269,7 +11269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11291,7 +11291,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11313,7 +11313,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11335,7 +11335,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11379,7 +11379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11401,7 +11401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11423,7 +11423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11445,7 +11445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11467,7 +11467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11489,7 +11489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11511,7 +11511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11533,7 +11533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11555,7 +11555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11577,7 +11577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11599,7 +11599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11621,7 +11621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11643,7 +11643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11665,7 +11665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11687,7 +11687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11709,7 +11709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11731,7 +11731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11753,7 +11753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11775,7 +11775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11797,7 +11797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11819,7 +11819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11841,7 +11841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11863,7 +11863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11885,7 +11885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11907,7 +11907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11929,7 +11929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11951,7 +11951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11973,7 +11973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11995,7 +11995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12017,7 +12017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12039,7 +12039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12061,7 +12061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12083,7 +12083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12105,7 +12105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12127,7 +12127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12149,7 +12149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12171,7 +12171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12193,7 +12193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12215,7 +12215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12237,7 +12237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12259,7 +12259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12281,7 +12281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12303,7 +12303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12325,7 +12325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12347,7 +12347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12369,7 +12369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12391,7 +12391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12413,7 +12413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12435,7 +12435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12457,7 +12457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12479,7 +12479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12501,7 +12501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12523,7 +12523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12545,7 +12545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12567,7 +12567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12589,7 +12589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12611,7 +12611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12633,7 +12633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12655,7 +12655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12677,7 +12677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12699,7 +12699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12721,7 +12721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12743,7 +12743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12765,7 +12765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12787,7 +12787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12809,7 +12809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12831,7 +12831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12853,7 +12853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12875,7 +12875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12897,7 +12897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12919,7 +12919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12941,7 +12941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12963,7 +12963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12985,7 +12985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13007,7 +13007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13029,7 +13029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13051,7 +13051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13073,7 +13073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13095,7 +13095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13117,7 +13117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13139,7 +13139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13161,7 +13161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13183,7 +13183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13205,7 +13205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13227,7 +13227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13249,7 +13249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13271,7 +13271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13293,7 +13293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13315,7 +13315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13337,7 +13337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13359,7 +13359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13381,7 +13381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13403,7 +13403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13425,7 +13425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13447,7 +13447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13469,7 +13469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13491,7 +13491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13513,7 +13513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13535,7 +13535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13557,7 +13557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13579,7 +13579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13601,7 +13601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13623,7 +13623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13645,7 +13645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13667,7 +13667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13689,7 +13689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13711,7 +13711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13733,7 +13733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13755,7 +13755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13777,7 +13777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13799,7 +13799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13821,7 +13821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13843,7 +13843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13865,7 +13865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13887,7 +13887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13909,7 +13909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13931,7 +13931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13953,7 +13953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13975,7 +13975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13997,7 +13997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14019,7 +14019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14041,7 +14041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14063,7 +14063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14085,7 +14085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14107,7 +14107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14129,7 +14129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14151,7 +14151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14173,7 +14173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14195,7 +14195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14217,7 +14217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14239,7 +14239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14261,7 +14261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14283,7 +14283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14305,7 +14305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14327,7 +14327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14349,7 +14349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14371,7 +14371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14393,7 +14393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14415,7 +14415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14437,7 +14437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14459,7 +14459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14481,7 +14481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14503,7 +14503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14525,7 +14525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14547,7 +14547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14569,7 +14569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14591,7 +14591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14613,7 +14613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14635,7 +14635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14657,7 +14657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14679,7 +14679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14701,7 +14701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14723,7 +14723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14745,7 +14745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14767,7 +14767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14789,7 +14789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14811,7 +14811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14833,7 +14833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14855,7 +14855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14877,7 +14877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14899,7 +14899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14921,7 +14921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14943,7 +14943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14965,7 +14965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14987,7 +14987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15009,7 +15009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15031,7 +15031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15053,7 +15053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15075,7 +15075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15097,7 +15097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15119,7 +15119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15141,7 +15141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15163,7 +15163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15185,7 +15185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15207,7 +15207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15229,7 +15229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15251,7 +15251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15273,7 +15273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15295,7 +15295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15317,7 +15317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15339,7 +15339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15361,7 +15361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15383,7 +15383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15405,7 +15405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15427,7 +15427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15449,7 +15449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15471,7 +15471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15493,7 +15493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15515,7 +15515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15537,7 +15537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15559,7 +15559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15581,7 +15581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15603,7 +15603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15625,7 +15625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15647,7 +15647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15669,7 +15669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15691,7 +15691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15713,7 +15713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15735,7 +15735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15757,7 +15757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15779,7 +15779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15801,7 +15801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15823,7 +15823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15845,7 +15845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15867,7 +15867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15889,7 +15889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15911,7 +15911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15933,7 +15933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15955,7 +15955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15977,7 +15977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -15999,7 +15999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16021,7 +16021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16043,7 +16043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16065,7 +16065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16087,7 +16087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16109,7 +16109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16131,7 +16131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16153,7 +16153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16175,7 +16175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16197,7 +16197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16219,7 +16219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16241,7 +16241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16263,7 +16263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16285,7 +16285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16307,7 +16307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16329,7 +16329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16351,7 +16351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16373,7 +16373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16395,7 +16395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16417,7 +16417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16439,7 +16439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16461,7 +16461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16483,7 +16483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16505,7 +16505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16527,7 +16527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16549,7 +16549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16571,7 +16571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16593,7 +16593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16615,7 +16615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16637,7 +16637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16659,37 +16659,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16710,13 +16710,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.453125" customWidth="1"/>
+    <col min="2" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16725,14 +16725,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16741,7 +16741,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16789,7 +16789,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16833,7 +16833,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16855,7 +16855,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16877,13 +16877,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16892,7 +16892,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>42</v>
       </c>
@@ -16901,12 +16901,12 @@
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -16915,7 +16915,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
@@ -16932,7 +16932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -16956,7 +16956,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
@@ -16980,7 +16980,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>2</v>
       </c>
@@ -17004,7 +17004,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -17028,7 +17028,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -17054,7 +17054,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>9</v>
       </c>
@@ -17064,7 +17064,7 @@
       <c r="E13" s="59"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>10</v>
       </c>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>0</v>
       </c>
@@ -17104,7 +17104,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>1</v>
       </c>
@@ -17126,7 +17126,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>2</v>
       </c>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>3</v>
       </c>
@@ -17170,7 +17170,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -17178,7 +17178,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -17186,7 +17186,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -17196,7 +17196,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>9</v>
       </c>
@@ -17206,7 +17206,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>10</v>
       </c>
@@ -17222,7 +17222,7 @@
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>0</v>
       </c>
@@ -17242,7 +17242,7 @@
       <c r="F24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>1</v>
       </c>
@@ -17262,7 +17262,7 @@
       <c r="F25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>2</v>
       </c>
@@ -17282,7 +17282,7 @@
       <c r="F26" s="22"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>3</v>
       </c>
@@ -17302,7 +17302,7 @@
       <c r="F27" s="22"/>
       <c r="H27" s="22"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
@@ -17311,7 +17311,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -17322,7 +17322,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>9</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="F30" s="58"/>
       <c r="G30" s="59"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>10</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
@@ -17391,7 +17391,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>21</v>
       </c>
@@ -17426,7 +17426,7 @@
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>2</v>
       </c>
@@ -17461,7 +17461,7 @@
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>3</v>
       </c>
@@ -17518,193 +17518,193 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
     <col min="37" max="37" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="str" cm="1">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="str">
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>25</v>
       </c>
@@ -18008,7 +18008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>1</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>2</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>3</v>
       </c>
@@ -18530,7 +18530,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4</v>
       </c>
@@ -18704,7 +18704,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>5</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>6</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>7</v>
       </c>
@@ -19226,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>8</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>9</v>
       </c>
@@ -19574,7 +19574,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="42">
         <v>10</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>11</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="42">
         <v>12</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="42">
         <v>13</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>14</v>
       </c>
@@ -20444,7 +20444,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="42">
         <v>15</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="42">
         <v>16</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="42">
         <v>17</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="42">
         <v>18</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="42">
         <v>19</v>
       </c>
@@ -21314,7 +21314,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="42">
         <v>20</v>
       </c>
@@ -21488,7 +21488,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>21</v>
       </c>
@@ -21662,7 +21662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="42">
         <v>22</v>
       </c>
@@ -21836,7 +21836,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>23</v>
       </c>
@@ -22010,7 +22010,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="42">
         <v>24</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="42">
         <v>25</v>
       </c>
@@ -22358,7 +22358,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="42">
         <v>26</v>
       </c>
@@ -22532,7 +22532,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>27</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="42">
         <v>28</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>29</v>
       </c>
@@ -23054,7 +23054,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="42">
         <v>30</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>36</v>
       </c>
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23433,7 +23433,7 @@
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection algorithmName="SHA-512" hashValue="yvv3wbdeRzmlM4bzNOO2apq3mx/qVFX0Msifl9YhWgFuHibBrkknge+pGfxzSIcsAi5W1vdadtYqYf6xCYTqPg==" saltValue="d9XYKX9Q0BviUTprb1l8GA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23454,7 +23454,7 @@
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>336550</xdr:colOff>
+                <xdr:colOff>333375</xdr:colOff>
                 <xdr:row>21</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-29
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D89A1B-3A78-412F-9B6B-3982D22484D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F048A9-4875-470F-B55B-047BC7DD3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29445" yWindow="1755" windowWidth="26715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2503,17 +2503,17 @@
           <cell r="H32">
             <v>46050</v>
           </cell>
-          <cell r="I32" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J32" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K32" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L32" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I32">
+            <v>3.95E-2</v>
+          </cell>
+          <cell r="J32">
+            <v>4.2900000000000001E-2</v>
+          </cell>
+          <cell r="K32">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L32">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="33">
@@ -8560,7 +8560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9206,21 +9206,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
       </c>
-      <c r="B31" s="17" t="str">
+      <c r="B31" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I32</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C31" s="47" t="str">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C31" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J32</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D31" s="47" t="str">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="D31" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K32</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E31" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E31" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L32</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17527,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-30
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F048A9-4875-470F-B55B-047BC7DD3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263E3217-2534-493C-A933-A008D7336603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29445" yWindow="1755" windowWidth="26715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31365" yWindow="1695" windowWidth="23610" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2520,17 +2520,17 @@
           <cell r="H33">
             <v>46051</v>
           </cell>
-          <cell r="I33" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J33" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K33" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L33" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I33">
+            <v>3.95E-2</v>
+          </cell>
+          <cell r="J33">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K33">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L33">
+            <v>4.8300000000000003E-2</v>
           </cell>
         </row>
         <row r="34">
@@ -8560,7 +8560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9228,21 +9228,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
       </c>
-      <c r="B32" s="17" t="str">
+      <c r="B32" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I33</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C32" s="47" t="str">
+        <v>3.95E-2</v>
+      </c>
+      <c r="C32" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J33</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D32" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D32" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K33</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E32" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E32" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L33</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17527,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="str" cm="1">
+      <c r="A1" s="61" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="67"/>
-      <c r="M1" s="65" t="str" cm="1">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="63"/>
+      <c r="M1" s="61" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="67"/>
-      <c r="Y1" s="65" t="str" cm="1">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="63"/>
+      <c r="Y1" s="61" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AK1" s="65" t="str" cm="1">
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AK1" s="61" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="67"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="63"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="str">
+      <c r="A2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="M2" s="61" t="str">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="66"/>
+      <c r="M2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63"/>
-      <c r="Y2" s="61" t="str">
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="66"/>
+      <c r="Y2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="63"/>
-      <c r="AK2" s="61" t="str">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="66"/>
+      <c r="AK2" s="64" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="63"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
+      <c r="AT2" s="65"/>
+      <c r="AU2" s="66"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="64" t="s">
+      <c r="N3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="Z3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64" t="s">
+      <c r="AL3" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23404,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="N3:W3"/>
     <mergeCell ref="AK1:AU1"/>
     <mergeCell ref="AK2:AU2"/>
     <mergeCell ref="AL3:AU3"/>
     <mergeCell ref="Y1:AI1"/>
     <mergeCell ref="Y2:AI2"/>
     <mergeCell ref="Z3:AI3"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:W1"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="N3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-01-31
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263E3217-2534-493C-A933-A008D7336603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374FEDB5-FF42-49EA-9C93-0C852A7A3774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31365" yWindow="1695" windowWidth="23610" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000%"/>
   </numFmts>
@@ -573,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,13 +585,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C46718A9-9EF5-4C7E-9DA1-DE598EFA01D5}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2537,17 +2539,17 @@
           <cell r="H34">
             <v>46052</v>
           </cell>
-          <cell r="I34" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J34" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K34" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L34" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I34">
+            <v>3.9399999999999998E-2</v>
+          </cell>
+          <cell r="J34">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K34">
+            <v>4.5600000000000002E-2</v>
+          </cell>
+          <cell r="L34">
+            <v>4.8399999999999999E-2</v>
           </cell>
         </row>
         <row r="35">
@@ -8560,7 +8562,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9250,21 +9252,21 @@
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
       </c>
-      <c r="B33" s="17" t="str">
+      <c r="B33" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I34</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C33" s="47" t="str">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="C33" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J34</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D33" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D33" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K34</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E33" s="5" t="str">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="E33" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L34</f>
-        <v xml:space="preserve"> </v>
+        <v>4.8399999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -17527,182 +17529,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="str" cm="1">
+      <c r="A1" s="65" t="str" cm="1">
         <f t="array" ref="A1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q1 VM - V Table X"</f>
         <v>2026 Q1 VM - V Table X</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="63"/>
-      <c r="M1" s="61" t="str" cm="1">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="67"/>
+      <c r="M1" s="65" t="str" cm="1">
         <f t="array" ref="M1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q2 VM - 22 Table X"</f>
         <v>2026 Q2 VM - 22 Table X</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="63"/>
-      <c r="Y1" s="61" t="str" cm="1">
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="67"/>
+      <c r="Y1" s="65" t="str" cm="1">
         <f t="array" ref="Y1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q3 VM - 22 Table X"</f>
         <v>2026 Q3 VM - 22 Table X</v>
       </c>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AK1" s="61" t="str" cm="1">
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AK1" s="65" t="str" cm="1">
         <f t="array" ref="AK1">TEXT([1]!Year_of_Valuation,"0000")&amp; " Q4 VM - 22 Table X"</f>
         <v>2026 Q4 VM - 22 Table X</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="63"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="67"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="str">
+      <c r="A2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation-1,10,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation-1,12,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>10/1/2025 thru 12/31/2025 Quarterly Average Spread Data</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="66"/>
-      <c r="M2" s="64" t="str">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="M2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>1/1/2026 thru 3/31/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="66"/>
-      <c r="Y2" s="64" t="str">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
+      <c r="Y2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>4/1/2026 thru 6/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
-      <c r="AK2" s="64" t="str">
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="63"/>
+      <c r="AK2" s="61" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy")&amp; " thru " &amp; TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")&amp; " Quarterly Average Spread Data"</f>
         <v>7/1/2026 thru 9/30/2026 Quarterly Average Spread Data</v>
       </c>
-      <c r="AL2" s="65"/>
-      <c r="AM2" s="65"/>
-      <c r="AN2" s="65"/>
-      <c r="AO2" s="65"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
-      <c r="AT2" s="65"/>
-      <c r="AU2" s="66"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="63"/>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
       <c r="M3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="67" t="s">
+      <c r="N3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
       <c r="Y3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Z3" s="67" t="s">
+      <c r="Z3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="67"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="67"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
       <c r="AK3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="67" t="s">
+      <c r="AL3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="67"/>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="67"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
@@ -23404,18 +23406,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AK2:AU2"/>
+    <mergeCell ref="AL3:AU3"/>
+    <mergeCell ref="Y1:AI1"/>
+    <mergeCell ref="Y2:AI2"/>
+    <mergeCell ref="Z3:AI3"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="M2:W2"/>
     <mergeCell ref="N3:W3"/>
-    <mergeCell ref="AK1:AU1"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AL3:AU3"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="Y2:AI2"/>
-    <mergeCell ref="Z3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
📊 Update NAIC content history - 2026-02-03
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
+++ b/docs/content_history/pbr-2026-vmv-nonjumbo-jumbo-valuation-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374FEDB5-FF42-49EA-9C93-0C852A7A3774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6E73EE-CA7E-4F96-9261-DD83E0BFF13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Jumbo Rates" sheetId="4" r:id="rId1"/>
@@ -573,6 +573,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,15 +592,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -627,7 +627,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>336550</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
@@ -2556,51 +2556,51 @@
           <cell r="H35">
             <v>46053</v>
           </cell>
-          <cell r="I35" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J35" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K35" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L35" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I35">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J35">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K35">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L35">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="36">
           <cell r="H36">
             <v>46054</v>
           </cell>
-          <cell r="I36" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J36" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K36" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L36" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I36">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J36">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K36">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L36">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="37">
           <cell r="H37">
             <v>46055</v>
           </cell>
-          <cell r="I37" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="J37" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="K37" t="str">
-            <v xml:space="preserve"> </v>
-          </cell>
-          <cell r="L37" t="str">
-            <v xml:space="preserve"> </v>
+          <cell r="I37">
+            <v>3.9300000000000002E-2</v>
+          </cell>
+          <cell r="J37">
+            <v>4.2999999999999997E-2</v>
+          </cell>
+          <cell r="K37">
+            <v>4.5699999999999998E-2</v>
+          </cell>
+          <cell r="L37">
+            <v>4.8500000000000001E-2</v>
           </cell>
         </row>
         <row r="38">
@@ -8562,19 +8562,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="46"/>
       <c r="B1" s="51" t="s">
         <v>4</v>
@@ -8583,7 +8583,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="53"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -8592,7 +8592,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H5</f>
         <v>46023</v>
@@ -8631,7 +8631,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H6</f>
         <v>46024</v>
@@ -8653,7 +8653,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H7</f>
         <v>46025</v>
@@ -8675,7 +8675,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H8</f>
         <v>46026</v>
@@ -8697,7 +8697,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H9</f>
         <v>46027</v>
@@ -8719,7 +8719,7 @@
         <v>4.8800000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H10</f>
         <v>46028</v>
@@ -8741,7 +8741,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H11</f>
         <v>46029</v>
@@ -8763,7 +8763,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H12</f>
         <v>46030</v>
@@ -8785,7 +8785,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H13</f>
         <v>46031</v>
@@ -8807,7 +8807,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H14</f>
         <v>46032</v>
@@ -8829,7 +8829,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H15</f>
         <v>46033</v>
@@ -8851,7 +8851,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H16</f>
         <v>46034</v>
@@ -8873,7 +8873,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H17</f>
         <v>46035</v>
@@ -8895,7 +8895,7 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H18</f>
         <v>46036</v>
@@ -8917,7 +8917,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H19</f>
         <v>46037</v>
@@ -8939,7 +8939,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H20</f>
         <v>46038</v>
@@ -8961,7 +8961,7 @@
         <v>4.7899999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H21</f>
         <v>46039</v>
@@ -8983,7 +8983,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H22</f>
         <v>46040</v>
@@ -9005,7 +9005,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H23</f>
         <v>46041</v>
@@ -9027,7 +9027,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H24</f>
         <v>46042</v>
@@ -9049,7 +9049,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H25</f>
         <v>46043</v>
@@ -9071,7 +9071,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H26</f>
         <v>46044</v>
@@ -9093,7 +9093,7 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H27</f>
         <v>46045</v>
@@ -9115,7 +9115,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H28</f>
         <v>46046</v>
@@ -9137,7 +9137,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H29</f>
         <v>46047</v>
@@ -9159,7 +9159,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H30</f>
         <v>46048</v>
@@ -9181,7 +9181,7 @@
         <v>4.82E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H31</f>
         <v>46049</v>
@@ -9203,7 +9203,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H32</f>
         <v>46050</v>
@@ -9225,7 +9225,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H33</f>
         <v>46051</v>
@@ -9247,7 +9247,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H34</f>
         <v>46052</v>
@@ -9269,73 +9269,73 @@
         <v>4.8399999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H35</f>
         <v>46053</v>
       </c>
-      <c r="B34" s="17" t="str">
+      <c r="B34" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I35</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C34" s="47" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C34" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J35</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D34" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D34" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K35</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E34" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E34" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L35</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H36</f>
         <v>46054</v>
       </c>
-      <c r="B35" s="17" t="str">
+      <c r="B35" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I36</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C35" s="47" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C35" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J36</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D35" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D35" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K36</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E35" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E35" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L36</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H37</f>
         <v>46055</v>
       </c>
-      <c r="B36" s="17" t="str">
+      <c r="B36" s="17">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!I37</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C36" s="47" t="str">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="C36" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!J37</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D36" s="47" t="str">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D36" s="47">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!K37</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E36" s="5" t="str">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="E36" s="5">
         <f ca="1">'[1]Jumbo Bus Date to PDD'!L37</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H38</f>
         <v>46056</v>
@@ -9357,7 +9357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H39</f>
         <v>46057</v>
@@ -9379,7 +9379,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H40</f>
         <v>46058</v>
@@ -9401,7 +9401,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H41</f>
         <v>46059</v>
@@ -9423,7 +9423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H42</f>
         <v>46060</v>
@@ -9445,7 +9445,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H43</f>
         <v>46061</v>
@@ -9467,7 +9467,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H44</f>
         <v>46062</v>
@@ -9489,7 +9489,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H45</f>
         <v>46063</v>
@@ -9511,7 +9511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H46</f>
         <v>46064</v>
@@ -9533,7 +9533,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H47</f>
         <v>46065</v>
@@ -9555,7 +9555,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H48</f>
         <v>46066</v>
@@ -9577,7 +9577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H49</f>
         <v>46067</v>
@@ -9599,7 +9599,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H50</f>
         <v>46068</v>
@@ -9621,7 +9621,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H51</f>
         <v>46069</v>
@@ -9643,7 +9643,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H52</f>
         <v>46070</v>
@@ -9665,7 +9665,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H53</f>
         <v>46071</v>
@@ -9687,7 +9687,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H54</f>
         <v>46072</v>
@@ -9709,7 +9709,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H55</f>
         <v>46073</v>
@@ -9731,7 +9731,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H56</f>
         <v>46074</v>
@@ -9753,7 +9753,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H57</f>
         <v>46075</v>
@@ -9775,7 +9775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H58</f>
         <v>46076</v>
@@ -9797,7 +9797,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H59</f>
         <v>46077</v>
@@ -9819,7 +9819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H60</f>
         <v>46078</v>
@@ -9841,7 +9841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H61</f>
         <v>46079</v>
@@ -9863,7 +9863,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H62</f>
         <v>46080</v>
@@ -9885,7 +9885,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H63</f>
         <v>46081</v>
@@ -9907,7 +9907,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H64</f>
         <v>46082</v>
@@ -9929,7 +9929,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H65</f>
         <v>46083</v>
@@ -9951,7 +9951,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H66</f>
         <v>46084</v>
@@ -9973,7 +9973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H67</f>
         <v>46085</v>
@@ -9995,7 +9995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H68</f>
         <v>46086</v>
@@ -10017,7 +10017,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H69</f>
         <v>46087</v>
@@ -10039,7 +10039,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H70</f>
         <v>46088</v>
@@ -10061,7 +10061,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H71</f>
         <v>46089</v>
@@ -10083,7 +10083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H72</f>
         <v>46090</v>
@@ -10105,7 +10105,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H73</f>
         <v>46091</v>
@@ -10127,7 +10127,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H74</f>
         <v>46092</v>
@@ -10149,7 +10149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H75</f>
         <v>46093</v>
@@ -10171,7 +10171,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H76</f>
         <v>46094</v>
@@ -10193,7 +10193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H77</f>
         <v>46095</v>
@@ -10215,7 +10215,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H78</f>
         <v>46096</v>
@@ -10237,7 +10237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H79</f>
         <v>46097</v>
@@ -10259,7 +10259,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H80</f>
         <v>46098</v>
@@ -10281,7 +10281,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H81</f>
         <v>46099</v>
@@ -10303,7 +10303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H82</f>
         <v>46100</v>
@@ -10325,7 +10325,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H83</f>
         <v>46101</v>
@@ -10347,7 +10347,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H84</f>
         <v>46102</v>
@@ -10369,7 +10369,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H85</f>
         <v>46103</v>
@@ -10391,7 +10391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H86</f>
         <v>46104</v>
@@ -10413,7 +10413,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H87</f>
         <v>46105</v>
@@ -10435,7 +10435,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H88</f>
         <v>46106</v>
@@ -10457,7 +10457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H89</f>
         <v>46107</v>
@@ -10479,7 +10479,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H90</f>
         <v>46108</v>
@@ -10501,7 +10501,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H91</f>
         <v>46109</v>
@@ -10523,7 +10523,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H92</f>
         <v>46110</v>
@@ -10545,7 +10545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H93</f>
         <v>46111</v>
@@ -10567,7 +10567,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H94</f>
         <v>46112</v>
@@ -10589,7 +10589,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H95</f>
         <v>46113</v>
@@ -10611,7 +10611,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H96</f>
         <v>46114</v>
@@ -10633,7 +10633,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H97</f>
         <v>46115</v>
@@ -10655,7 +10655,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H98</f>
         <v>46116</v>
@@ -10677,7 +10677,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H99</f>
         <v>46117</v>
@@ -10699,7 +10699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H100</f>
         <v>46118</v>
@@ -10721,7 +10721,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H101</f>
         <v>46119</v>
@@ -10743,7 +10743,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H102</f>
         <v>46120</v>
@@ -10765,7 +10765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H103</f>
         <v>46121</v>
@@ -10787,7 +10787,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H104</f>
         <v>46122</v>
@@ -10809,7 +10809,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H105</f>
         <v>46123</v>
@@ -10831,7 +10831,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H106</f>
         <v>46124</v>
@@ -10853,7 +10853,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H107</f>
         <v>46125</v>
@@ -10875,7 +10875,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H108</f>
         <v>46126</v>
@@ -10897,7 +10897,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H109</f>
         <v>46127</v>
@@ -10919,7 +10919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H110</f>
         <v>46128</v>
@@ -10941,7 +10941,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H111</f>
         <v>46129</v>
@@ -10963,7 +10963,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H112</f>
         <v>46130</v>
@@ -10985,7 +10985,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H113</f>
         <v>46131</v>
@@ -11007,7 +11007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H114</f>
         <v>46132</v>
@@ -11029,7 +11029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H115</f>
         <v>46133</v>
@@ -11051,7 +11051,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H116</f>
         <v>46134</v>
@@ -11073,7 +11073,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H117</f>
         <v>46135</v>
@@ -11095,7 +11095,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H118</f>
         <v>46136</v>
@@ -11117,7 +11117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H119</f>
         <v>46137</v>
@@ -11139,7 +11139,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H120</f>
         <v>46138</v>
@@ -11161,7 +11161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H121</f>
         <v>46139</v>
@@ -11183,7 +11183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H122</f>
         <v>46140</v>
@@ -11205,7 +11205,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H123</f>
         <v>46141</v>
@@ -11227,7 +11227,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H124</f>
         <v>46142</v>
@@ -11249,7 +11249,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H125</f>
         <v>46143</v>
@@ -11271,7 +11271,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H126</f>
         <v>46144</v>
@@ -11293,7 +11293,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H127</f>
         <v>46145</v>
@@ -11315,7 +11315,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H128</f>
         <v>46146</v>
@@ -11337,7 +11337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H129</f>
         <v>46147</v>
@@ -11359,7 +11359,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H130</f>
         <v>46148</v>
@@ -11381,7 +11381,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H131</f>
         <v>46149</v>
@@ -11403,7 +11403,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H132</f>
         <v>46150</v>
@@ -11425,7 +11425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H133</f>
         <v>46151</v>
@@ -11447,7 +11447,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H134</f>
         <v>46152</v>
@@ -11469,7 +11469,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H135</f>
         <v>46153</v>
@@ -11491,7 +11491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H136</f>
         <v>46154</v>
@@ -11513,7 +11513,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H137</f>
         <v>46155</v>
@@ -11535,7 +11535,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H138</f>
         <v>46156</v>
@@ -11557,7 +11557,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H139</f>
         <v>46157</v>
@@ -11579,7 +11579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H140</f>
         <v>46158</v>
@@ -11601,7 +11601,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H141</f>
         <v>46159</v>
@@ -11623,7 +11623,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H142</f>
         <v>46160</v>
@@ -11645,7 +11645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H143</f>
         <v>46161</v>
@@ -11667,7 +11667,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H144</f>
         <v>46162</v>
@@ -11689,7 +11689,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H145</f>
         <v>46163</v>
@@ -11711,7 +11711,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H146</f>
         <v>46164</v>
@@ -11733,7 +11733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H147</f>
         <v>46165</v>
@@ -11755,7 +11755,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H148</f>
         <v>46166</v>
@@ -11777,7 +11777,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H149</f>
         <v>46167</v>
@@ -11799,7 +11799,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H150</f>
         <v>46168</v>
@@ -11821,7 +11821,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H151</f>
         <v>46169</v>
@@ -11843,7 +11843,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H152</f>
         <v>46170</v>
@@ -11865,7 +11865,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H153</f>
         <v>46171</v>
@@ -11887,7 +11887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H154</f>
         <v>46172</v>
@@ -11909,7 +11909,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H155</f>
         <v>46173</v>
@@ -11931,7 +11931,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H156</f>
         <v>46174</v>
@@ -11953,7 +11953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H157</f>
         <v>46175</v>
@@ -11975,7 +11975,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H158</f>
         <v>46176</v>
@@ -11997,7 +11997,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H159</f>
         <v>46177</v>
@@ -12019,7 +12019,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H160</f>
         <v>46178</v>
@@ -12041,7 +12041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H161</f>
         <v>46179</v>
@@ -12063,7 +12063,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H162</f>
         <v>46180</v>
@@ -12085,7 +12085,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H163</f>
         <v>46181</v>
@@ -12107,7 +12107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H164</f>
         <v>46182</v>
@@ -12129,7 +12129,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H165</f>
         <v>46183</v>
@@ -12151,7 +12151,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H166</f>
         <v>46184</v>
@@ -12173,7 +12173,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H167</f>
         <v>46185</v>
@@ -12195,7 +12195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H168</f>
         <v>46186</v>
@@ -12217,7 +12217,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H169</f>
         <v>46187</v>
@@ -12239,7 +12239,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H170</f>
         <v>46188</v>
@@ -12261,7 +12261,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H171</f>
         <v>46189</v>
@@ -12283,7 +12283,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H172</f>
         <v>46190</v>
@@ -12305,7 +12305,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H173</f>
         <v>46191</v>
@@ -12327,7 +12327,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H174</f>
         <v>46192</v>
@@ -12349,7 +12349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H175</f>
         <v>46193</v>
@@ -12371,7 +12371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H176</f>
         <v>46194</v>
@@ -12393,7 +12393,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H177</f>
         <v>46195</v>
@@ -12415,7 +12415,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H178</f>
         <v>46196</v>
@@ -12437,7 +12437,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H179</f>
         <v>46197</v>
@@ -12459,7 +12459,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H180</f>
         <v>46198</v>
@@ -12481,7 +12481,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H181</f>
         <v>46199</v>
@@ -12503,7 +12503,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H182</f>
         <v>46200</v>
@@ -12525,7 +12525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H183</f>
         <v>46201</v>
@@ -12547,7 +12547,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H184</f>
         <v>46202</v>
@@ -12569,7 +12569,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H185</f>
         <v>46203</v>
@@ -12591,7 +12591,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H186</f>
         <v>46204</v>
@@ -12613,7 +12613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H187</f>
         <v>46205</v>
@@ -12635,7 +12635,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H188</f>
         <v>46206</v>
@@ -12657,7 +12657,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H189</f>
         <v>46207</v>
@@ -12679,7 +12679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H190</f>
         <v>46208</v>
@@ -12701,7 +12701,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H191</f>
         <v>46209</v>
@@ -12723,7 +12723,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H192</f>
         <v>46210</v>
@@ -12745,7 +12745,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H193</f>
         <v>46211</v>
@@ -12767,7 +12767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H194</f>
         <v>46212</v>
@@ -12789,7 +12789,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H195</f>
         <v>46213</v>
@@ -12811,7 +12811,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H196</f>
         <v>46214</v>
@@ -12833,7 +12833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H197</f>
         <v>46215</v>
@@ -12855,7 +12855,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H198</f>
         <v>46216</v>
@@ -12877,7 +12877,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H199</f>
         <v>46217</v>
@@ -12899,7 +12899,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H200</f>
         <v>46218</v>
@@ -12921,7 +12921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H201</f>
         <v>46219</v>
@@ -12943,7 +12943,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H202</f>
         <v>46220</v>
@@ -12965,7 +12965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H203</f>
         <v>46221</v>
@@ -12987,7 +12987,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H204</f>
         <v>46222</v>
@@ -13009,7 +13009,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H205</f>
         <v>46223</v>
@@ -13031,7 +13031,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H206</f>
         <v>46224</v>
@@ -13053,7 +13053,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H207</f>
         <v>46225</v>
@@ -13075,7 +13075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H208</f>
         <v>46226</v>
@@ -13097,7 +13097,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H209</f>
         <v>46227</v>
@@ -13119,7 +13119,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H210</f>
         <v>46228</v>
@@ -13141,7 +13141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H211</f>
         <v>46229</v>
@@ -13163,7 +13163,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H212</f>
         <v>46230</v>
@@ -13185,7 +13185,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H213</f>
         <v>46231</v>
@@ -13207,7 +13207,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H214</f>
         <v>46232</v>
@@ -13229,7 +13229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H215</f>
         <v>46233</v>
@@ -13251,7 +13251,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H216</f>
         <v>46234</v>
@@ -13273,7 +13273,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H217</f>
         <v>46235</v>
@@ -13295,7 +13295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H218</f>
         <v>46236</v>
@@ -13317,7 +13317,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H219</f>
         <v>46237</v>
@@ -13339,7 +13339,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H220</f>
         <v>46238</v>
@@ -13361,7 +13361,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H221</f>
         <v>46239</v>
@@ -13383,7 +13383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H222</f>
         <v>46240</v>
@@ -13405,7 +13405,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H223</f>
         <v>46241</v>
@@ -13427,7 +13427,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H224</f>
         <v>46242</v>
@@ -13449,7 +13449,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H225</f>
         <v>46243</v>
@@ -13471,7 +13471,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H226</f>
         <v>46244</v>
@@ -13493,7 +13493,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H227</f>
         <v>46245</v>
@@ -13515,7 +13515,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H228</f>
         <v>46246</v>
@@ -13537,7 +13537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H229</f>
         <v>46247</v>
@@ -13559,7 +13559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H230</f>
         <v>46248</v>
@@ -13581,7 +13581,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H231</f>
         <v>46249</v>
@@ -13603,7 +13603,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H232</f>
         <v>46250</v>
@@ -13625,7 +13625,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H233</f>
         <v>46251</v>
@@ -13647,7 +13647,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H234</f>
         <v>46252</v>
@@ -13669,7 +13669,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H235</f>
         <v>46253</v>
@@ -13691,7 +13691,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H236</f>
         <v>46254</v>
@@ -13713,7 +13713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H237</f>
         <v>46255</v>
@@ -13735,7 +13735,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H238</f>
         <v>46256</v>
@@ -13757,7 +13757,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H239</f>
         <v>46257</v>
@@ -13779,7 +13779,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H240</f>
         <v>46258</v>
@@ -13801,7 +13801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H241</f>
         <v>46259</v>
@@ -13823,7 +13823,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H242</f>
         <v>46260</v>
@@ -13845,7 +13845,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H243</f>
         <v>46261</v>
@@ -13867,7 +13867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H244</f>
         <v>46262</v>
@@ -13889,7 +13889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H245</f>
         <v>46263</v>
@@ -13911,7 +13911,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H246</f>
         <v>46264</v>
@@ -13933,7 +13933,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H247</f>
         <v>46265</v>
@@ -13955,7 +13955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H248</f>
         <v>46266</v>
@@ -13977,7 +13977,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H249</f>
         <v>46267</v>
@@ -13999,7 +13999,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H250</f>
         <v>46268</v>
@@ -14021,7 +14021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H251</f>
         <v>46269</v>
@@ -14043,7 +14043,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H252</f>
         <v>46270</v>
@@ -14065,7 +14065,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H253</f>
         <v>46271</v>
@@ -14087,7 +14087,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H254</f>
         <v>46272</v>
@@ -14109,7 +14109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H255</f>
         <v>46273</v>
@@ -14131,7 +14131,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H256</f>
         <v>46274</v>
@@ -14153,7 +14153,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H257</f>
         <v>46275</v>
@@ -14175,7 +14175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H258</f>
         <v>46276</v>
@@ -14197,7 +14197,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H259</f>
         <v>46277</v>
@@ -14219,7 +14219,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H260</f>
         <v>46278</v>
@@ -14241,7 +14241,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H261</f>
         <v>46279</v>
@@ -14263,7 +14263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H262</f>
         <v>46280</v>
@@ -14285,7 +14285,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H263</f>
         <v>46281</v>
@@ -14307,7 +14307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H264</f>
         <v>46282</v>
@@ -14329,7 +14329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H265</f>
         <v>46283</v>
@@ -14351,7 +14351,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H266</f>
         <v>46284</v>
@@ -14373,7 +14373,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H267</f>
         <v>46285</v>
@@ -14395,7 +14395,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H268</f>
         <v>46286</v>
@@ -14417,7 +14417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H269</f>
         <v>46287</v>
@@ -14439,7 +14439,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H270</f>
         <v>46288</v>
@@ -14461,7 +14461,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H271</f>
         <v>46289</v>
@@ -14483,7 +14483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H272</f>
         <v>46290</v>
@@ -14505,7 +14505,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H273</f>
         <v>46291</v>
@@ -14527,7 +14527,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H274</f>
         <v>46292</v>
@@ -14549,7 +14549,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H275</f>
         <v>46293</v>
@@ -14571,7 +14571,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H276</f>
         <v>46294</v>
@@ -14593,7 +14593,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H277</f>
         <v>46295</v>
@@ -14615,7 +14615,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H278</f>
         <v>46296</v>
@@ -14637,7 +14637,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H279</f>
         <v>46297</v>
@@ -14659,7 +14659,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H280</f>
         <v>46298</v>
@@ -14681,7 +14681,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H281</f>
         <v>46299</v>
@@ -14703,7 +14703,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H282</f>
         <v>46300</v>
@@ -14725,7 +14725,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H283</f>
         <v>46301</v>
@@ -14747,7 +14747,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H284</f>
         <v>46302</v>
@@ -14769,7 +14769,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H285</f>
         <v>46303</v>
@@ -14791,7 +14791,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H286</f>
         <v>46304</v>
@@ -14813,7 +14813,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H287</f>
         <v>46305</v>
@@ -14835,7 +14835,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H288</f>
         <v>46306</v>
@@ -14857,7 +14857,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H289</f>
         <v>46307</v>
@@ -14879,7 +14879,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H290</f>
         <v>46308</v>
@@ -14901,7 +14901,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H291</f>
         <v>46309</v>
@@ -14923,7 +14923,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H292</f>
         <v>46310</v>
@@ -14945,7 +14945,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H293</f>
         <v>46311</v>
@@ -14967,7 +14967,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H294</f>
         <v>46312</v>
@@ -14989,7 +14989,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H295</f>
         <v>46313</v>
@@ -15011,7 +15011,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H296</f>
         <v>46314</v>
@@ -15033,7 +15033,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H297</f>
         <v>46315</v>
@@ -15055,7 +15055,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H298</f>
         <v>46316</v>
@@ -15077,7 +15077,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H299</f>
         <v>46317</v>
@@ -15099,7 +15099,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H300</f>
         <v>46318</v>
@@ -15121,7 +15121,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H301</f>
         <v>46319</v>
@@ -15143,7 +15143,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H302</f>
         <v>46320</v>
@@ -15165,7 +15165,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H303</f>
         <v>46321</v>
@@ -15187,7 +15187,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H304</f>
         <v>46322</v>
@@ -15209,7 +15209,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H305</f>
         <v>46323</v>
@@ -15231,7 +15231,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H306</f>
         <v>46324</v>
@@ -15253,7 +15253,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H307</f>
         <v>46325</v>
@@ -15275,7 +15275,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H308</f>
         <v>46326</v>
@@ -15297,7 +15297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H309</f>
         <v>46327</v>
@@ -15319,7 +15319,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H310</f>
         <v>46328</v>
@@ -15341,7 +15341,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H311</f>
         <v>46329</v>
@@ -15363,7 +15363,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H312</f>
         <v>46330</v>
@@ -15385,7 +15385,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H313</f>
         <v>46331</v>
@@ -15407,7 +15407,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H314</f>
         <v>46332</v>
@@ -15429,7 +15429,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H315</f>
         <v>46333</v>
@@ -15451,7 +15451,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H316</f>
         <v>46334</v>
@@ -15473,7 +15473,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H317</f>
         <v>46335</v>
@@ -15495,7 +15495,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H318</f>
         <v>46336</v>
@@ -15517,7 +15517,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H319</f>
         <v>46337</v>
@@ -15539,7 +15539,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H320</f>
         <v>46338</v>
@@ -15561,7 +15561,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H321</f>
         <v>46339</v>
@@ -15583,7 +15583,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H322</f>
         <v>46340</v>
@@ -15605,7 +15605,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H323</f>
         <v>46341</v>
@@ -15627,7 +15627,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H324</f>
         <v>46342</v>
@@ -15649,7 +15649,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H325</f>
         <v>46343</v>
@@ -15671,7 +15671,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H326</f>
         <v>46344</v>
@@ -15693,7 +15693,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H327</f>
         <v>46345</v>
@@ -15715,7 +15715,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H328</f>
         <v>46346</v>
@@ -15737,7 +15737,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H329</f>
         <v>46347</v>
@@ -15759,7 +15759,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H330</f>
         <v>46348</v>
@@ -15781,7 +15781,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H331</f>
         <v>46349</v>
@@ -15803,7 +15803,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H332</f>
         <v>46350</v>
@@ -15825,7 +15825,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H333</f>
         <v>46351</v>
@@ -15847,7 +15847,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H334</f>
         <v>46352</v>
@@ -15869,7 +15869,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H335</f>
         <v>46353</v>
@@ -15891,7 +15891,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H336</f>
         <v>46354</v>
@@ -15913,7 +15913,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H337</f>
         <v>46355</v>
@@ -15935,7 +15935,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H338</f>
         <v>46356</v>
@@ -15957,7 +15957,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H339</f>
         <v>46357</v>
@@ -15979,7 +15979,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H340</f>
         <v>46358</v>
@@ -16001,7 +16001,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H341</f>
         <v>46359</v>
@@ -16023,7 +16023,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H342</f>
         <v>46360</v>
@@ -16045,7 +16045,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H343</f>
         <v>46361</v>
@@ -16067,7 +16067,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H344</f>
         <v>46362</v>
@@ -16089,7 +16089,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H345</f>
         <v>46363</v>
@@ -16111,7 +16111,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H346</f>
         <v>46364</v>
@@ -16133,7 +16133,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H347</f>
         <v>46365</v>
@@ -16155,7 +16155,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H348</f>
         <v>46366</v>
@@ -16177,7 +16177,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H349</f>
         <v>46367</v>
@@ -16199,7 +16199,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H350</f>
         <v>46368</v>
@@ -16221,7 +16221,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H351</f>
         <v>46369</v>
@@ -16243,7 +16243,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H352</f>
         <v>46370</v>
@@ -16265,7 +16265,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H353</f>
         <v>46371</v>
@@ -16287,7 +16287,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H354</f>
         <v>46372</v>
@@ -16309,7 +16309,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H355</f>
         <v>46373</v>
@@ -16331,7 +16331,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H356</f>
         <v>46374</v>
@@ -16353,7 +16353,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H357</f>
         <v>46375</v>
@@ -16375,7 +16375,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H358</f>
         <v>46376</v>
@@ -16397,7 +16397,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H359</f>
         <v>46377</v>
@@ -16419,7 +16419,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H360</f>
         <v>46378</v>
@@ -16441,7 +16441,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H361</f>
         <v>46379</v>
@@ -16463,7 +16463,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H362</f>
         <v>46380</v>
@@ -16485,7 +16485,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H363</f>
         <v>46381</v>
@@ -16507,7 +16507,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H364</f>
         <v>46382</v>
@@ -16529,7 +16529,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H365</f>
         <v>46383</v>
@@ -16551,7 +16551,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H366</f>
         <v>46384</v>
@@ -16573,7 +16573,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H367</f>
         <v>46385</v>
@@ -16595,7 +16595,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H368</f>
         <v>46386</v>
@@ -16617,7 +16617,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" s="15">
         <f>'[1]Jumbo Bus Date to PDD'!H369</f>
         <v>46387</v>
@@ -16639,7 +16639,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" s="45">
         <f>'[1]Jumbo Bus Date to PDD'!H370</f>
         <v>46388</v>
@@ -16661,37 +16661,37 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" s="15"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" s="15"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" s="15"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" s="15"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" s="15"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" s="15"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" s="15"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" s="15"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" s="15"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" s="15"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" s="15"/>
     </row>
   </sheetData>
@@ -16712,13 +16712,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
@@ -16727,14 +16727,14 @@
       <c r="D1" s="55"/>
       <c r="E1" s="56"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -16743,7 +16743,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -16752,7 +16752,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
@@ -16769,7 +16769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,1,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,3,31),"m/d/yyyy")</f>
         <v>1/1/2026 - 3/31/2026</v>
@@ -16791,7 +16791,7 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,4,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,6,30),"m/d/yyyy")</f>
         <v>4/1/2026 - 6/30/2026</v>
@@ -16813,7 +16813,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,7,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,9,30),"m/d/yyyy")</f>
         <v>7/1/2026 - 9/30/2026</v>
@@ -16835,7 +16835,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="str">
         <f>TEXT(DATE([1]!Year_of_Valuation,10,1),"m/d/yyyy") &amp;" - " &amp;TEXT(DATE([1]!Year_of_Valuation,12,31),"m/d/yyyy")</f>
         <v>10/1/2026 - 12/31/2026</v>
@@ -16857,7 +16857,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="48"/>
     </row>
   </sheetData>
@@ -16879,13 +16879,13 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
@@ -16894,7 +16894,7 @@
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" sp